<commit_message>
commiting the updated code
</commit_message>
<xml_diff>
--- a/DataDriven/src/test/resources/excel/testdata.xlsx
+++ b/DataDriven/src/test/resources/excel/testdata.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
   <si>
     <t>Firstname</t>
   </si>
@@ -57,6 +57,9 @@
     <t>asud</t>
   </si>
   <si>
+    <t>Customer added succlly</t>
+  </si>
+  <si>
     <t>rupesh</t>
   </si>
   <si>
@@ -66,6 +69,9 @@
     <t>fchxh</t>
   </si>
   <si>
+    <t>N</t>
+  </si>
+  <si>
     <t>vankatesh</t>
   </si>
   <si>
@@ -73,9 +79,6 @@
   </si>
   <si>
     <t>sxakbv</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t>rahul</t>
@@ -122,10 +125,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -143,16 +146,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -183,14 +210,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -220,61 +247,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -295,55 +298,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -355,48 +466,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -404,78 +479,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -500,6 +503,41 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -543,15 +581,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -567,21 +596,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -590,173 +604,171 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1079,7 +1091,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="4"/>
@@ -1088,16 +1100,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -1105,16 +1117,16 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E2" t="s">
@@ -1122,61 +1134,69 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="E3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="C4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="B5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="C6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="E6" t="s">
         <v>9</v>
       </c>
@@ -1193,37 +1213,40 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="2"/>
+  <cols>
+    <col min="3" max="3" width="32.8888888888889" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="C1" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="2" ht="28.8" spans="1:3">
+      <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>28</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1247,7 +1270,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -1255,7 +1278,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -1263,7 +1286,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -1271,7 +1294,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>

</xml_diff>